<commit_message>
2024-06-07 Marco teóricoa la mitad.
</commit_message>
<xml_diff>
--- a/DIA A DIA/Organización.xlsx
+++ b/DIA A DIA/Organización.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjime\Documents\ESTUDIOS\GRADO MATEMATICAS\4-CUARTO\TFG\A.A.A.C\GIT\DIA A DIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B76AB0-9685-4CFB-8A02-33D174A557E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2EA9C0-8523-4D66-8D4B-D66E6BE1AFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="68">
   <si>
     <t>LUNES - 27</t>
   </si>
@@ -212,9 +212,6 @@
     <t>RNN KDD</t>
   </si>
   <si>
-    <t>RBM KDD</t>
-  </si>
-  <si>
     <t>Escribir resultados</t>
   </si>
   <si>
@@ -225,6 +222,24 @@
   </si>
   <si>
     <t>Marco teórico</t>
+  </si>
+  <si>
+    <t>Funciones de activación y pérdida subrayadas</t>
+  </si>
+  <si>
+    <t>Validación cruzada y problemas datos.</t>
+  </si>
+  <si>
+    <t>Regularización</t>
+  </si>
+  <si>
+    <t>Escribir section 3</t>
+  </si>
+  <si>
+    <t>Escribir 3</t>
+  </si>
+  <si>
+    <t>Métricas y verificación test (matiz confusión)</t>
   </si>
 </sst>
 </file>
@@ -279,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,29 +302,25 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -594,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="63" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="63" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,7 +780,7 @@
       <c r="A14" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>50</v>
       </c>
       <c r="C14" s="1"/>
@@ -783,7 +794,7 @@
       <c r="A15" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -836,7 +847,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="9" t="s">
         <v>4</v>
       </c>
       <c r="F19" s="1"/>
@@ -850,7 +861,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -862,7 +873,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -874,7 +885,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -886,7 +897,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -898,7 +909,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1076,9 +1087,11 @@
       <c r="F40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>58</v>
+      <c r="G40" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -1090,8 +1103,8 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
@@ -1102,8 +1115,8 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
@@ -1114,8 +1127,8 @@
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="8"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
@@ -1126,8 +1139,8 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
@@ -1136,22 +1149,24 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="5"/>
+      <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="5"/>
+      <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+      <c r="G46" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" s="8"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
@@ -1160,10 +1175,10 @@
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="5"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
@@ -1172,10 +1187,10 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="5"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="8"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
@@ -1184,7 +1199,7 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="5"/>
+      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -1196,7 +1211,7 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="5"/>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -1208,10 +1223,12 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="5"/>
+      <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="H51" s="8" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
@@ -1220,10 +1237,12 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="5"/>
+      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="G52" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" s="8"/>
     </row>
     <row r="53" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
@@ -1232,10 +1251,10 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="4"/>
+      <c r="E53" s="3"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
     </row>
     <row r="54" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
@@ -1244,10 +1263,10 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="3"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
     </row>
     <row r="55" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
@@ -1256,10 +1275,12 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="4"/>
+      <c r="E55" s="3"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="G55" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H55" s="8"/>
     </row>
     <row r="56" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
@@ -1268,9 +1289,9 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="4"/>
+      <c r="E56" s="3"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="G56" s="7"/>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1280,9 +1301,9 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="4"/>
+      <c r="E57" s="3"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
+      <c r="G57" s="7"/>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1292,9 +1313,9 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="4"/>
+      <c r="E58" s="3"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+      <c r="G58" s="7"/>
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -1304,7 +1325,7 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="5"/>
+      <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -1316,7 +1337,7 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="5"/>
+      <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -1328,7 +1349,7 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="5"/>
+      <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -1340,7 +1361,7 @@
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="5"/>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -1352,7 +1373,7 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="5"/>
+      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -1364,7 +1385,7 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="5"/>
+      <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -1376,7 +1397,7 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="5"/>
+      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -1388,19 +1409,10 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="5"/>
+      <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E69" s="6"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
@@ -1413,7 +1425,7 @@
       <c r="D70" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F70" s="1" t="s">
@@ -1433,8 +1445,8 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="10"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="4"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
@@ -1445,7 +1457,7 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="F72" s="10"/>
+      <c r="F72" s="4"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
@@ -1456,13 +1468,13 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="10"/>
-      <c r="F73" s="10"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
       <c r="G73" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -1472,8 +1484,8 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
     </row>
@@ -1484,13 +1496,13 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -1502,8 +1514,8 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="10"/>
-      <c r="F76" s="10"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
@@ -1514,8 +1526,8 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
@@ -1526,8 +1538,8 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
@@ -1538,8 +1550,8 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
@@ -1550,8 +1562,8 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
@@ -1562,8 +1574,8 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
@@ -1574,8 +1586,8 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
-      <c r="E82" s="10"/>
-      <c r="F82" s="10"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
@@ -1586,8 +1598,8 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
-      <c r="E83" s="10"/>
-      <c r="F83" s="10"/>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
@@ -1598,8 +1610,8 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
-      <c r="E84" s="10"/>
-      <c r="F84" s="10"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
@@ -1610,7 +1622,7 @@
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
-      <c r="E85" s="10"/>
+      <c r="E85" s="4"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
@@ -1622,7 +1634,7 @@
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
-      <c r="E86" s="10"/>
+      <c r="E86" s="4"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
@@ -1634,7 +1646,7 @@
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
-      <c r="E87" s="10"/>
+      <c r="E87" s="4"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
@@ -1646,7 +1658,7 @@
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
-      <c r="E88" s="10"/>
+      <c r="E88" s="4"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
@@ -1658,7 +1670,7 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
-      <c r="E89" s="10"/>
+      <c r="E89" s="4"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
@@ -1670,7 +1682,7 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
-      <c r="E90" s="10"/>
+      <c r="E90" s="4"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
@@ -1682,7 +1694,7 @@
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
-      <c r="E91" s="10"/>
+      <c r="E91" s="4"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
@@ -1694,7 +1706,7 @@
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
-      <c r="E92" s="10"/>
+      <c r="E92" s="4"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
@@ -1706,7 +1718,7 @@
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
-      <c r="E93" s="4"/>
+      <c r="E93" s="3"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
@@ -1718,7 +1730,7 @@
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
-      <c r="E94" s="5"/>
+      <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
@@ -1730,7 +1742,7 @@
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
-      <c r="E95" s="5"/>
+      <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
@@ -1742,7 +1754,7 @@
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
-      <c r="E96" s="5"/>
+      <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
@@ -1754,7 +1766,7 @@
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
-      <c r="E97" s="5"/>
+      <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
@@ -1766,7 +1778,7 @@
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
-      <c r="E98" s="5"/>
+      <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
@@ -1778,7 +1790,7 @@
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
-      <c r="E99" s="5"/>
+      <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
@@ -1790,7 +1802,7 @@
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
-      <c r="E100" s="5"/>
+      <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
@@ -1802,19 +1814,10 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
-      <c r="E101" s="5"/>
+      <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E102" s="6"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E103" s="6"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E104" s="6"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
@@ -1827,7 +1830,7 @@
       <c r="D105" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E105" s="5" t="s">
+      <c r="E105" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F105" s="1" t="s">
@@ -1847,9 +1850,9 @@
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="11" t="s">
-        <v>60</v>
+      <c r="E106" s="1"/>
+      <c r="F106" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
@@ -1861,8 +1864,8 @@
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="11"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="6"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
@@ -1870,35 +1873,35 @@
       <c r="A108" s="2">
         <v>0.375</v>
       </c>
-      <c r="B108" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D108" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E108" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F108" s="11"/>
+      <c r="B108" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F108" s="6"/>
       <c r="G108" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
@@ -1906,11 +1909,11 @@
       <c r="A110" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
-      <c r="E110" s="11"/>
-      <c r="F110" s="11"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
@@ -1918,11 +1921,11 @@
       <c r="A111" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B111" s="11"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="11"/>
-      <c r="E111" s="11"/>
-      <c r="F111" s="11"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
@@ -1930,11 +1933,11 @@
       <c r="A112" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B112" s="11"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="11"/>
-      <c r="E112" s="11"/>
-      <c r="F112" s="11"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
@@ -1942,11 +1945,11 @@
       <c r="A113" s="2">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B113" s="11"/>
-      <c r="C113" s="11"/>
-      <c r="D113" s="11"/>
-      <c r="E113" s="11"/>
-      <c r="F113" s="11"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
@@ -1954,11 +1957,11 @@
       <c r="A114" s="2">
         <v>0.5</v>
       </c>
-      <c r="B114" s="11"/>
-      <c r="C114" s="11"/>
-      <c r="D114" s="11"/>
-      <c r="E114" s="11"/>
-      <c r="F114" s="11"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
     </row>
@@ -1966,11 +1969,11 @@
       <c r="A115" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B115" s="11"/>
-      <c r="C115" s="11"/>
-      <c r="D115" s="11"/>
-      <c r="E115" s="11"/>
-      <c r="F115" s="11"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
@@ -1978,11 +1981,11 @@
       <c r="A116" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B116" s="11"/>
-      <c r="C116" s="11"/>
-      <c r="D116" s="11"/>
-      <c r="E116" s="11"/>
-      <c r="F116" s="11"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
@@ -1990,11 +1993,11 @@
       <c r="A117" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="11"/>
-      <c r="E117" s="11"/>
-      <c r="F117" s="11"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
@@ -2002,11 +2005,11 @@
       <c r="A118" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
@@ -2014,11 +2017,11 @@
       <c r="A119" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B119" s="11"/>
-      <c r="C119" s="11"/>
-      <c r="D119" s="11"/>
-      <c r="E119" s="11"/>
-      <c r="F119" s="11"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="6"/>
+      <c r="F119" s="6"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
@@ -2026,10 +2029,10 @@
       <c r="A120" s="2">
         <v>0.625</v>
       </c>
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-      <c r="E120" s="11"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="6"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="6"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
@@ -2038,10 +2041,10 @@
       <c r="A121" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="B121" s="11"/>
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
-      <c r="E121" s="11"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
@@ -2050,12 +2053,12 @@
       <c r="A122" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B122" s="11"/>
-      <c r="C122" s="11"/>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
       <c r="F122" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -2064,10 +2067,10 @@
       <c r="A123" s="2">
         <v>0.6875</v>
       </c>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
@@ -2076,10 +2079,10 @@
       <c r="A124" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B124" s="11"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
@@ -2088,10 +2091,10 @@
       <c r="A125" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="B125" s="11"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="6"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
@@ -2100,10 +2103,10 @@
       <c r="A126" s="2">
         <v>0.75</v>
       </c>
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
-      <c r="E126" s="11"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -2112,10 +2115,10 @@
       <c r="A127" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B127" s="11"/>
-      <c r="C127" s="11"/>
-      <c r="D127" s="11"/>
-      <c r="E127" s="11"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="6"/>
+      <c r="E127" s="6"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -2127,7 +2130,7 @@
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
-      <c r="E128" s="5"/>
+      <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -2139,7 +2142,7 @@
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
-      <c r="E129" s="5"/>
+      <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
@@ -2149,16 +2152,16 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -2171,7 +2174,7 @@
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
-      <c r="E131" s="5"/>
+      <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -2229,9 +2232,6 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E138" s="6"/>
-    </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="1"/>
       <c r="B139" s="1" t="s">
@@ -2243,7 +2243,7 @@
       <c r="D139" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E139" s="5" t="s">
+      <c r="E139" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F139" s="1" t="s">
@@ -2262,12 +2262,12 @@
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
-      <c r="D140" s="9" t="s">
+      <c r="D140" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E140" s="5"/>
-      <c r="F140" s="11" t="s">
-        <v>60</v>
+      <c r="E140" s="1"/>
+      <c r="F140" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
@@ -2278,9 +2278,9 @@
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
-      <c r="D141" s="9"/>
-      <c r="E141" s="5"/>
-      <c r="F141" s="11"/>
+      <c r="D141" s="5"/>
+      <c r="E141" s="1"/>
+      <c r="F141" s="6"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
     </row>
@@ -2288,17 +2288,17 @@
       <c r="A142" s="2">
         <v>0.375</v>
       </c>
-      <c r="B142" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C142" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D142" s="9"/>
-      <c r="E142" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F142" s="11"/>
+      <c r="B142" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C142" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D142" s="5"/>
+      <c r="E142" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F142" s="6"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
     </row>
@@ -2306,11 +2306,11 @@
       <c r="A143" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B143" s="11"/>
-      <c r="C143" s="11"/>
-      <c r="D143" s="9"/>
-      <c r="E143" s="11"/>
-      <c r="F143" s="11"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="5"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
     </row>
@@ -2318,11 +2318,11 @@
       <c r="A144" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B144" s="11"/>
-      <c r="C144" s="11"/>
-      <c r="D144" s="9"/>
-      <c r="E144" s="11"/>
-      <c r="F144" s="11"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="5"/>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
     </row>
@@ -2330,11 +2330,11 @@
       <c r="A145" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B145" s="11"/>
-      <c r="C145" s="11"/>
-      <c r="D145" s="9"/>
-      <c r="E145" s="11"/>
-      <c r="F145" s="11"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="5"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
     </row>
@@ -2342,11 +2342,11 @@
       <c r="A146" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B146" s="11"/>
-      <c r="C146" s="11"/>
-      <c r="D146" s="9"/>
-      <c r="E146" s="11"/>
-      <c r="F146" s="11"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="6"/>
+      <c r="D146" s="5"/>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
     </row>
@@ -2354,11 +2354,11 @@
       <c r="A147" s="2">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B147" s="11"/>
-      <c r="C147" s="11"/>
-      <c r="D147" s="9"/>
-      <c r="E147" s="11"/>
-      <c r="F147" s="11"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="6"/>
+      <c r="F147" s="6"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
     </row>
@@ -2366,11 +2366,11 @@
       <c r="A148" s="2">
         <v>0.5</v>
       </c>
-      <c r="B148" s="11"/>
-      <c r="C148" s="11"/>
-      <c r="D148" s="9"/>
-      <c r="E148" s="11"/>
-      <c r="F148" s="11"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="6"/>
+      <c r="F148" s="6"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
     </row>
@@ -2378,11 +2378,11 @@
       <c r="A149" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B149" s="11"/>
-      <c r="C149" s="11"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="6"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="6"/>
+      <c r="F149" s="6"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
     </row>
@@ -2390,11 +2390,11 @@
       <c r="A150" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B150" s="11"/>
-      <c r="C150" s="11"/>
-      <c r="D150" s="9"/>
-      <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="6"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="6"/>
+      <c r="F150" s="6"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
     </row>
@@ -2402,11 +2402,11 @@
       <c r="A151" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B151" s="11"/>
-      <c r="C151" s="11"/>
-      <c r="D151" s="9"/>
-      <c r="E151" s="11"/>
-      <c r="F151" s="11"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
     </row>
@@ -2414,11 +2414,11 @@
       <c r="A152" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B152" s="11"/>
-      <c r="C152" s="11"/>
-      <c r="D152" s="9"/>
-      <c r="E152" s="11"/>
-      <c r="F152" s="11"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="6"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="6"/>
+      <c r="F152" s="6"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
     </row>
@@ -2426,11 +2426,11 @@
       <c r="A153" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B153" s="11"/>
-      <c r="C153" s="11"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="11"/>
-      <c r="F153" s="11"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="6"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="6"/>
+      <c r="F153" s="6"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
     </row>
@@ -2438,10 +2438,10 @@
       <c r="A154" s="2">
         <v>0.625</v>
       </c>
-      <c r="B154" s="11"/>
-      <c r="C154" s="11"/>
-      <c r="D154" s="9"/>
-      <c r="E154" s="11"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="6"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="6"/>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
@@ -2450,10 +2450,10 @@
       <c r="A155" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="B155" s="11"/>
-      <c r="C155" s="11"/>
-      <c r="D155" s="9"/>
-      <c r="E155" s="11"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="6"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="6"/>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
@@ -2462,10 +2462,10 @@
       <c r="A156" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B156" s="11"/>
-      <c r="C156" s="11"/>
-      <c r="D156" s="9"/>
-      <c r="E156" s="11"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="6"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="6"/>
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
@@ -2474,10 +2474,10 @@
       <c r="A157" s="2">
         <v>0.6875</v>
       </c>
-      <c r="B157" s="11"/>
-      <c r="C157" s="11"/>
-      <c r="D157" s="9"/>
-      <c r="E157" s="11"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="6"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="6"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
@@ -2486,10 +2486,10 @@
       <c r="A158" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B158" s="11"/>
-      <c r="C158" s="11"/>
-      <c r="D158" s="9"/>
-      <c r="E158" s="11"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="6"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="6"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
@@ -2498,10 +2498,10 @@
       <c r="A159" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="B159" s="11"/>
-      <c r="C159" s="11"/>
-      <c r="D159" s="9"/>
-      <c r="E159" s="11"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="6"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="6"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
@@ -2510,10 +2510,10 @@
       <c r="A160" s="2">
         <v>0.75</v>
       </c>
-      <c r="B160" s="11"/>
-      <c r="C160" s="11"/>
-      <c r="D160" s="9"/>
-      <c r="E160" s="11"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="6"/>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
@@ -2522,10 +2522,10 @@
       <c r="A161" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B161" s="11"/>
-      <c r="C161" s="11"/>
-      <c r="D161" s="9"/>
-      <c r="E161" s="11"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="6"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="6"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
@@ -2536,8 +2536,8 @@
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
-      <c r="D162" s="9"/>
-      <c r="E162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="1"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
@@ -2548,8 +2548,8 @@
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
-      <c r="D163" s="9"/>
-      <c r="E163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="1"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
@@ -2560,8 +2560,8 @@
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
-      <c r="D164" s="9"/>
-      <c r="E164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="1"/>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
@@ -2572,8 +2572,8 @@
       </c>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
-      <c r="D165" s="9"/>
-      <c r="E165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="1"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
-      <c r="D166" s="9"/>
+      <c r="D166" s="5"/>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
-      <c r="D167" s="9"/>
+      <c r="D167" s="5"/>
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
-      <c r="D168" s="9"/>
+      <c r="D168" s="5"/>
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
@@ -2620,7 +2620,7 @@
       </c>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
-      <c r="D169" s="9"/>
+      <c r="D169" s="5"/>
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
@@ -2630,7 +2630,7 @@
       <c r="A170" s="2">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D170" s="9"/>
+      <c r="D170" s="5"/>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="1"/>
@@ -2643,7 +2643,7 @@
       <c r="D173" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E173" s="5" t="s">
+      <c r="E173" s="1" t="s">
         <v>40</v>
       </c>
       <c r="F173" s="1" t="s">
@@ -2660,20 +2660,20 @@
       <c r="A174" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B174" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C174" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D174" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E174" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F174" s="11" t="s">
-        <v>60</v>
+      <c r="B174" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
@@ -2682,11 +2682,11 @@
       <c r="A175" s="2">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B175" s="11"/>
-      <c r="C175" s="11"/>
-      <c r="D175" s="11"/>
-      <c r="E175" s="11"/>
-      <c r="F175" s="11"/>
+      <c r="B175" s="6"/>
+      <c r="C175" s="6"/>
+      <c r="D175" s="6"/>
+      <c r="E175" s="6"/>
+      <c r="F175" s="6"/>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
     </row>
@@ -2694,11 +2694,11 @@
       <c r="A176" s="2">
         <v>0.375</v>
       </c>
-      <c r="B176" s="11"/>
-      <c r="C176" s="11"/>
-      <c r="D176" s="11"/>
-      <c r="E176" s="11"/>
-      <c r="F176" s="11"/>
+      <c r="B176" s="6"/>
+      <c r="C176" s="6"/>
+      <c r="D176" s="6"/>
+      <c r="E176" s="6"/>
+      <c r="F176" s="6"/>
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
     </row>
@@ -2706,11 +2706,11 @@
       <c r="A177" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B177" s="11"/>
-      <c r="C177" s="11"/>
-      <c r="D177" s="11"/>
-      <c r="E177" s="11"/>
-      <c r="F177" s="11"/>
+      <c r="B177" s="6"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="6"/>
+      <c r="E177" s="6"/>
+      <c r="F177" s="6"/>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
     </row>
@@ -2718,11 +2718,11 @@
       <c r="A178" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B178" s="11"/>
-      <c r="C178" s="11"/>
-      <c r="D178" s="11"/>
-      <c r="E178" s="11"/>
-      <c r="F178" s="11"/>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6"/>
+      <c r="D178" s="6"/>
+      <c r="E178" s="6"/>
+      <c r="F178" s="6"/>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
     </row>
@@ -2730,11 +2730,11 @@
       <c r="A179" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B179" s="11"/>
-      <c r="C179" s="11"/>
-      <c r="D179" s="11"/>
-      <c r="E179" s="11"/>
-      <c r="F179" s="11"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
+      <c r="D179" s="6"/>
+      <c r="E179" s="6"/>
+      <c r="F179" s="6"/>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
     </row>
@@ -2742,11 +2742,11 @@
       <c r="A180" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B180" s="11"/>
-      <c r="C180" s="11"/>
-      <c r="D180" s="11"/>
-      <c r="E180" s="11"/>
-      <c r="F180" s="11"/>
+      <c r="B180" s="6"/>
+      <c r="C180" s="6"/>
+      <c r="D180" s="6"/>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6"/>
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
     </row>
@@ -2754,11 +2754,11 @@
       <c r="A181" s="2">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B181" s="11"/>
-      <c r="C181" s="11"/>
-      <c r="D181" s="11"/>
-      <c r="E181" s="11"/>
-      <c r="F181" s="11"/>
+      <c r="B181" s="6"/>
+      <c r="C181" s="6"/>
+      <c r="D181" s="6"/>
+      <c r="E181" s="6"/>
+      <c r="F181" s="6"/>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
     </row>
@@ -2766,11 +2766,11 @@
       <c r="A182" s="2">
         <v>0.5</v>
       </c>
-      <c r="B182" s="11"/>
-      <c r="C182" s="11"/>
-      <c r="D182" s="11"/>
-      <c r="E182" s="11"/>
-      <c r="F182" s="11"/>
+      <c r="B182" s="6"/>
+      <c r="C182" s="6"/>
+      <c r="D182" s="6"/>
+      <c r="E182" s="6"/>
+      <c r="F182" s="6"/>
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
     </row>
@@ -2778,11 +2778,11 @@
       <c r="A183" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B183" s="11"/>
-      <c r="C183" s="11"/>
-      <c r="D183" s="11"/>
-      <c r="E183" s="11"/>
-      <c r="F183" s="11"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
     </row>
@@ -2790,11 +2790,11 @@
       <c r="A184" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B184" s="11"/>
-      <c r="C184" s="11"/>
-      <c r="D184" s="11"/>
-      <c r="E184" s="11"/>
-      <c r="F184" s="11"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
+      <c r="E184" s="6"/>
+      <c r="F184" s="6"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
     </row>
@@ -2802,11 +2802,11 @@
       <c r="A185" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B185" s="11"/>
-      <c r="C185" s="11"/>
-      <c r="D185" s="11"/>
-      <c r="E185" s="11"/>
-      <c r="F185" s="11"/>
+      <c r="B185" s="6"/>
+      <c r="C185" s="6"/>
+      <c r="D185" s="6"/>
+      <c r="E185" s="6"/>
+      <c r="F185" s="6"/>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
     </row>
@@ -2814,11 +2814,11 @@
       <c r="A186" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B186" s="11"/>
-      <c r="C186" s="11"/>
-      <c r="D186" s="11"/>
-      <c r="E186" s="11"/>
-      <c r="F186" s="11"/>
+      <c r="B186" s="6"/>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="6"/>
+      <c r="F186" s="6"/>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
     </row>
@@ -2826,11 +2826,11 @@
       <c r="A187" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B187" s="11"/>
-      <c r="C187" s="11"/>
-      <c r="D187" s="11"/>
-      <c r="E187" s="11"/>
-      <c r="F187" s="11"/>
+      <c r="B187" s="6"/>
+      <c r="C187" s="6"/>
+      <c r="D187" s="6"/>
+      <c r="E187" s="6"/>
+      <c r="F187" s="6"/>
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
     </row>
@@ -2840,10 +2840,10 @@
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
-      <c r="D188" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E188" s="5"/>
+      <c r="D188" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E188" s="1"/>
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
@@ -2854,8 +2854,8 @@
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
-      <c r="D189" s="9"/>
-      <c r="E189" s="5"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="1"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
@@ -2866,8 +2866,8 @@
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
-      <c r="D190" s="9"/>
-      <c r="E190" s="4"/>
+      <c r="D190" s="5"/>
+      <c r="E190" s="3"/>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
@@ -2878,8 +2878,8 @@
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
-      <c r="D191" s="9"/>
-      <c r="E191" s="4"/>
+      <c r="D191" s="5"/>
+      <c r="E191" s="3"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
@@ -2890,8 +2890,8 @@
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
-      <c r="D192" s="9"/>
-      <c r="E192" s="4"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="3"/>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
@@ -2902,8 +2902,8 @@
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
-      <c r="D193" s="9"/>
-      <c r="E193" s="4"/>
+      <c r="D193" s="5"/>
+      <c r="E193" s="3"/>
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
@@ -2914,8 +2914,8 @@
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
-      <c r="D194" s="9"/>
-      <c r="E194" s="4"/>
+      <c r="D194" s="5"/>
+      <c r="E194" s="3"/>
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
@@ -2926,8 +2926,8 @@
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
-      <c r="D195" s="9"/>
-      <c r="E195" s="4"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="3"/>
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
@@ -2938,8 +2938,8 @@
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
-      <c r="D196" s="9"/>
-      <c r="E196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="1"/>
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
@@ -2950,8 +2950,8 @@
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
-      <c r="D197" s="9"/>
-      <c r="E197" s="5"/>
+      <c r="D197" s="5"/>
+      <c r="E197" s="1"/>
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
@@ -2962,8 +2962,8 @@
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
-      <c r="D198" s="9"/>
-      <c r="E198" s="5"/>
+      <c r="D198" s="5"/>
+      <c r="E198" s="1"/>
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
@@ -2974,8 +2974,8 @@
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
-      <c r="D199" s="9"/>
-      <c r="E199" s="5"/>
+      <c r="D199" s="5"/>
+      <c r="E199" s="1"/>
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
-      <c r="D200" s="9"/>
+      <c r="D200" s="5"/>
       <c r="E200" s="1"/>
       <c r="F200" s="1"/>
       <c r="G200" s="1"/>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
-      <c r="D201" s="9"/>
+      <c r="D201" s="5"/>
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
       <c r="G201" s="1"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
-      <c r="D202" s="9"/>
+      <c r="D202" s="5"/>
       <c r="E202" s="1"/>
       <c r="F202" s="1"/>
       <c r="G202" s="1"/>
@@ -3022,7 +3022,7 @@
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
-      <c r="D203" s="9"/>
+      <c r="D203" s="5"/>
       <c r="E203" s="1"/>
       <c r="F203" s="1"/>
       <c r="G203" s="1"/>
@@ -3032,10 +3032,10 @@
       <c r="A204" s="2">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D204" s="9"/>
+      <c r="D204" s="5"/>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D205" s="9"/>
+      <c r="D205" s="5"/>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F207" s="1"/>
@@ -3058,7 +3058,7 @@
       <c r="D209" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E209" s="5" t="s">
+      <c r="E209" s="1" t="s">
         <v>47</v>
       </c>
       <c r="F209" s="1"/>
@@ -3069,17 +3069,17 @@
       <c r="A210" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B210" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C210" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D210" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E210" s="11" t="s">
-        <v>60</v>
+      <c r="B210" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C210" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D210" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E210" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="F210" s="1"/>
       <c r="G210" s="1"/>
@@ -3089,10 +3089,10 @@
       <c r="A211" s="2">
         <v>0.35416666666666669</v>
       </c>
-      <c r="B211" s="11"/>
-      <c r="C211" s="11"/>
-      <c r="D211" s="11"/>
-      <c r="E211" s="11"/>
+      <c r="B211" s="6"/>
+      <c r="C211" s="6"/>
+      <c r="D211" s="6"/>
+      <c r="E211" s="6"/>
       <c r="F211" s="1"/>
       <c r="G211" s="1"/>
       <c r="H211" s="1"/>
@@ -3101,10 +3101,10 @@
       <c r="A212" s="2">
         <v>0.375</v>
       </c>
-      <c r="B212" s="11"/>
-      <c r="C212" s="11"/>
-      <c r="D212" s="11"/>
-      <c r="E212" s="11"/>
+      <c r="B212" s="6"/>
+      <c r="C212" s="6"/>
+      <c r="D212" s="6"/>
+      <c r="E212" s="6"/>
       <c r="F212" s="1"/>
       <c r="G212" s="1"/>
       <c r="H212" s="1"/>
@@ -3113,10 +3113,10 @@
       <c r="A213" s="2">
         <v>0.39583333333333331</v>
       </c>
-      <c r="B213" s="11"/>
-      <c r="C213" s="11"/>
-      <c r="D213" s="11"/>
-      <c r="E213" s="11"/>
+      <c r="B213" s="6"/>
+      <c r="C213" s="6"/>
+      <c r="D213" s="6"/>
+      <c r="E213" s="6"/>
       <c r="F213" s="1"/>
       <c r="G213" s="1"/>
       <c r="H213" s="1"/>
@@ -3125,10 +3125,10 @@
       <c r="A214" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B214" s="11"/>
-      <c r="C214" s="11"/>
-      <c r="D214" s="11"/>
-      <c r="E214" s="11"/>
+      <c r="B214" s="6"/>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="E214" s="6"/>
       <c r="F214" s="1"/>
       <c r="G214" s="1"/>
       <c r="H214" s="1"/>
@@ -3137,10 +3137,10 @@
       <c r="A215" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B215" s="11"/>
-      <c r="C215" s="11"/>
-      <c r="D215" s="11"/>
-      <c r="E215" s="11"/>
+      <c r="B215" s="6"/>
+      <c r="C215" s="6"/>
+      <c r="D215" s="6"/>
+      <c r="E215" s="6"/>
       <c r="F215" s="1"/>
       <c r="G215" s="1"/>
       <c r="H215" s="1"/>
@@ -3149,10 +3149,10 @@
       <c r="A216" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B216" s="11"/>
-      <c r="C216" s="11"/>
-      <c r="D216" s="11"/>
-      <c r="E216" s="11"/>
+      <c r="B216" s="6"/>
+      <c r="C216" s="6"/>
+      <c r="D216" s="6"/>
+      <c r="E216" s="6"/>
       <c r="F216" s="1"/>
       <c r="G216" s="1"/>
       <c r="H216" s="1"/>
@@ -3161,10 +3161,10 @@
       <c r="A217" s="2">
         <v>0.47916666666666669</v>
       </c>
-      <c r="B217" s="11"/>
-      <c r="C217" s="11"/>
-      <c r="D217" s="11"/>
-      <c r="E217" s="11"/>
+      <c r="B217" s="6"/>
+      <c r="C217" s="6"/>
+      <c r="D217" s="6"/>
+      <c r="E217" s="6"/>
       <c r="F217" s="1"/>
       <c r="G217" s="1"/>
       <c r="H217" s="1"/>
@@ -3173,10 +3173,10 @@
       <c r="A218" s="2">
         <v>0.5</v>
       </c>
-      <c r="B218" s="11"/>
-      <c r="C218" s="11"/>
-      <c r="D218" s="11"/>
-      <c r="E218" s="11"/>
+      <c r="B218" s="6"/>
+      <c r="C218" s="6"/>
+      <c r="D218" s="6"/>
+      <c r="E218" s="6"/>
       <c r="F218" s="1"/>
       <c r="G218" s="1"/>
       <c r="H218" s="1"/>
@@ -3185,10 +3185,10 @@
       <c r="A219" s="2">
         <v>0.52083333333333337</v>
       </c>
-      <c r="B219" s="11"/>
-      <c r="C219" s="11"/>
-      <c r="D219" s="11"/>
-      <c r="E219" s="11"/>
+      <c r="B219" s="6"/>
+      <c r="C219" s="6"/>
+      <c r="D219" s="6"/>
+      <c r="E219" s="6"/>
       <c r="F219" s="1"/>
       <c r="G219" s="1"/>
       <c r="H219" s="1"/>
@@ -3197,10 +3197,10 @@
       <c r="A220" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B220" s="11"/>
-      <c r="C220" s="11"/>
-      <c r="D220" s="11"/>
-      <c r="E220" s="11"/>
+      <c r="B220" s="6"/>
+      <c r="C220" s="6"/>
+      <c r="D220" s="6"/>
+      <c r="E220" s="6"/>
       <c r="F220" s="1"/>
       <c r="G220" s="1"/>
       <c r="H220" s="1"/>
@@ -3209,10 +3209,10 @@
       <c r="A221" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B221" s="11"/>
-      <c r="C221" s="11"/>
-      <c r="D221" s="11"/>
-      <c r="E221" s="11"/>
+      <c r="B221" s="6"/>
+      <c r="C221" s="6"/>
+      <c r="D221" s="6"/>
+      <c r="E221" s="6"/>
       <c r="F221" s="1"/>
       <c r="G221" s="1"/>
       <c r="H221" s="1"/>
@@ -3221,10 +3221,10 @@
       <c r="A222" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B222" s="11"/>
-      <c r="C222" s="11"/>
-      <c r="D222" s="11"/>
-      <c r="E222" s="11"/>
+      <c r="B222" s="6"/>
+      <c r="C222" s="6"/>
+      <c r="D222" s="6"/>
+      <c r="E222" s="6"/>
       <c r="F222" s="1"/>
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
@@ -3233,10 +3233,10 @@
       <c r="A223" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="B223" s="11"/>
-      <c r="C223" s="11"/>
-      <c r="D223" s="11"/>
-      <c r="E223" s="11"/>
+      <c r="B223" s="6"/>
+      <c r="C223" s="6"/>
+      <c r="D223" s="6"/>
+      <c r="E223" s="6"/>
       <c r="F223" s="1"/>
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
@@ -3245,14 +3245,14 @@
       <c r="A224" s="2">
         <v>0.625</v>
       </c>
-      <c r="B224" s="8" t="s">
+      <c r="B224" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C224" s="1"/>
-      <c r="D224" s="9" t="s">
+      <c r="D224" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E224" s="9"/>
+      <c r="E224" s="5"/>
       <c r="F224" s="1"/>
       <c r="G224" s="1"/>
       <c r="H224" s="1"/>
@@ -3261,10 +3261,10 @@
       <c r="A225" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="B225" s="8"/>
+      <c r="B225" s="7"/>
       <c r="C225" s="1"/>
-      <c r="D225" s="9"/>
-      <c r="E225" s="9"/>
+      <c r="D225" s="5"/>
+      <c r="E225" s="5"/>
       <c r="F225" s="1"/>
       <c r="G225" s="1"/>
       <c r="H225" s="1"/>
@@ -3273,10 +3273,10 @@
       <c r="A226" s="2">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B226" s="8"/>
+      <c r="B226" s="7"/>
       <c r="C226" s="1"/>
-      <c r="D226" s="9"/>
-      <c r="E226" s="9"/>
+      <c r="D226" s="5"/>
+      <c r="E226" s="5"/>
       <c r="F226" s="1"/>
       <c r="G226" s="1"/>
       <c r="H226" s="1"/>
@@ -3285,10 +3285,10 @@
       <c r="A227" s="2">
         <v>0.6875</v>
       </c>
-      <c r="B227" s="8"/>
+      <c r="B227" s="7"/>
       <c r="C227" s="1"/>
-      <c r="D227" s="9"/>
-      <c r="E227" s="9"/>
+      <c r="D227" s="5"/>
+      <c r="E227" s="5"/>
       <c r="F227" s="1"/>
       <c r="G227" s="1"/>
       <c r="H227" s="1"/>
@@ -3297,10 +3297,10 @@
       <c r="A228" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B228" s="8"/>
+      <c r="B228" s="7"/>
       <c r="C228" s="1"/>
-      <c r="D228" s="9"/>
-      <c r="E228" s="9"/>
+      <c r="D228" s="5"/>
+      <c r="E228" s="5"/>
       <c r="F228" s="1"/>
       <c r="G228" s="1"/>
       <c r="H228" s="1"/>
@@ -3309,10 +3309,10 @@
       <c r="A229" s="2">
         <v>0.72916666666666663</v>
       </c>
-      <c r="B229" s="8"/>
+      <c r="B229" s="7"/>
       <c r="C229" s="1"/>
-      <c r="D229" s="9"/>
-      <c r="E229" s="9"/>
+      <c r="D229" s="5"/>
+      <c r="E229" s="5"/>
       <c r="F229" s="1"/>
       <c r="G229" s="1"/>
       <c r="H229" s="1"/>
@@ -3321,10 +3321,10 @@
       <c r="A230" s="2">
         <v>0.75</v>
       </c>
-      <c r="B230" s="8"/>
+      <c r="B230" s="7"/>
       <c r="C230" s="1"/>
-      <c r="D230" s="9"/>
-      <c r="E230" s="9"/>
+      <c r="D230" s="5"/>
+      <c r="E230" s="5"/>
       <c r="F230" s="1"/>
       <c r="G230" s="1"/>
       <c r="H230" s="1"/>
@@ -3333,10 +3333,10 @@
       <c r="A231" s="2">
         <v>0.77083333333333337</v>
       </c>
-      <c r="B231" s="8"/>
+      <c r="B231" s="7"/>
       <c r="C231" s="1"/>
-      <c r="D231" s="9"/>
-      <c r="E231" s="9"/>
+      <c r="D231" s="5"/>
+      <c r="E231" s="5"/>
       <c r="F231" s="1"/>
       <c r="G231" s="1"/>
       <c r="H231" s="1"/>
@@ -3345,10 +3345,10 @@
       <c r="A232" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B232" s="8"/>
+      <c r="B232" s="7"/>
       <c r="C232" s="1"/>
-      <c r="D232" s="9"/>
-      <c r="E232" s="9"/>
+      <c r="D232" s="5"/>
+      <c r="E232" s="5"/>
       <c r="F232" s="1"/>
       <c r="G232" s="1"/>
       <c r="H232" s="1"/>
@@ -3357,10 +3357,10 @@
       <c r="A233" s="2">
         <v>0.8125</v>
       </c>
-      <c r="B233" s="8"/>
+      <c r="B233" s="7"/>
       <c r="C233" s="1"/>
-      <c r="D233" s="9"/>
-      <c r="E233" s="9"/>
+      <c r="D233" s="5"/>
+      <c r="E233" s="5"/>
       <c r="F233" s="1"/>
       <c r="G233" s="1"/>
       <c r="H233" s="1"/>
@@ -3369,10 +3369,10 @@
       <c r="A234" s="2">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B234" s="8"/>
+      <c r="B234" s="7"/>
       <c r="C234" s="1"/>
-      <c r="D234" s="9"/>
-      <c r="E234" s="9"/>
+      <c r="D234" s="5"/>
+      <c r="E234" s="5"/>
       <c r="F234" s="1"/>
       <c r="G234" s="1"/>
       <c r="H234" s="1"/>
@@ -3381,10 +3381,10 @@
       <c r="A235" s="2">
         <v>0.85416666666666663</v>
       </c>
-      <c r="B235" s="8"/>
+      <c r="B235" s="7"/>
       <c r="C235" s="1"/>
-      <c r="D235" s="9"/>
-      <c r="E235" s="9"/>
+      <c r="D235" s="5"/>
+      <c r="E235" s="5"/>
       <c r="F235" s="1"/>
       <c r="G235" s="1"/>
       <c r="H235" s="1"/>
@@ -3393,10 +3393,10 @@
       <c r="A236" s="2">
         <v>0.875</v>
       </c>
-      <c r="B236" s="8"/>
+      <c r="B236" s="7"/>
       <c r="C236" s="1"/>
-      <c r="D236" s="9"/>
-      <c r="E236" s="9"/>
+      <c r="D236" s="5"/>
+      <c r="E236" s="5"/>
       <c r="F236" s="1"/>
       <c r="G236" s="1"/>
       <c r="H236" s="1"/>
@@ -3405,10 +3405,10 @@
       <c r="A237" s="2">
         <v>0.89583333333333337</v>
       </c>
-      <c r="B237" s="8"/>
+      <c r="B237" s="7"/>
       <c r="C237" s="1"/>
-      <c r="D237" s="9"/>
-      <c r="E237" s="9"/>
+      <c r="D237" s="5"/>
+      <c r="E237" s="5"/>
       <c r="F237" s="1"/>
       <c r="G237" s="1"/>
       <c r="H237" s="1"/>
@@ -3417,40 +3417,40 @@
       <c r="A238" s="2">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B238" s="8"/>
+      <c r="B238" s="7"/>
       <c r="C238" s="1"/>
-      <c r="D238" s="9"/>
-      <c r="E238" s="9"/>
+      <c r="D238" s="5"/>
+      <c r="E238" s="5"/>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A239" s="2">
         <v>0.9375</v>
       </c>
-      <c r="B239" s="8"/>
+      <c r="B239" s="7"/>
       <c r="C239" s="1"/>
-      <c r="D239" s="9"/>
-      <c r="E239" s="9"/>
+      <c r="D239" s="5"/>
+      <c r="E239" s="5"/>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A240" s="2">
         <v>0.95833333333333337</v>
       </c>
-      <c r="B240" s="8"/>
-      <c r="D240" s="9"/>
-      <c r="E240" s="9"/>
+      <c r="B240" s="7"/>
+      <c r="D240" s="5"/>
+      <c r="E240" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="D224:E240"/>
-    <mergeCell ref="C210:C223"/>
-    <mergeCell ref="B210:B223"/>
-    <mergeCell ref="D210:D223"/>
-    <mergeCell ref="E210:E223"/>
-    <mergeCell ref="D174:D187"/>
-    <mergeCell ref="D188:D205"/>
-    <mergeCell ref="B224:B240"/>
-    <mergeCell ref="C142:C161"/>
-    <mergeCell ref="E142:E161"/>
+  <mergeCells count="30">
+    <mergeCell ref="H40:H48"/>
+    <mergeCell ref="H51:H55"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D140:D170"/>
+    <mergeCell ref="B142:B161"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="G40:G44"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="G55:G58"/>
     <mergeCell ref="F106:F119"/>
     <mergeCell ref="F140:F153"/>
     <mergeCell ref="B174:B187"/>
@@ -3461,10 +3461,16 @@
     <mergeCell ref="C108:C127"/>
     <mergeCell ref="D108:D127"/>
     <mergeCell ref="E108:E127"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D140:D170"/>
-    <mergeCell ref="B142:B161"/>
-    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="D174:D187"/>
+    <mergeCell ref="D188:D205"/>
+    <mergeCell ref="B224:B240"/>
+    <mergeCell ref="C142:C161"/>
+    <mergeCell ref="E142:E161"/>
+    <mergeCell ref="D224:E240"/>
+    <mergeCell ref="C210:C223"/>
+    <mergeCell ref="B210:B223"/>
+    <mergeCell ref="D210:D223"/>
+    <mergeCell ref="E210:E223"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>